<commit_message>
feat: add matchsvr gamesvr
</commit_message>
<xml_diff>
--- a/gameconf/xlsx/enum.xlsx
+++ b/gameconf/xlsx/enum.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>E|游戏类型-无|GameType|None|0</t>
   </si>
@@ -54,46 +54,16 @@
     <t>E|货币类型-金币|CoinType|Coin|1</t>
   </si>
   <si>
-    <t>E|赛事类型-SNG|MatchType|SNG|1</t>
-  </si>
-  <si>
     <t>E|环境类型-测试|EnvType|Develop|1</t>
   </si>
   <si>
-    <t>E|游戏类型-德州SHORT|GameType|Short|2</t>
-  </si>
-  <si>
     <t>E|房间类型-中级|RoomType|Middle|2</t>
   </si>
   <si>
-    <t>E|货币类型-ACE|CoinType|Ace|2</t>
-  </si>
-  <si>
     <t>E|环境类型-发布|EnvType|Release|2</t>
   </si>
   <si>
-    <t>E|游戏类型-德州AOF|GameType|Aof|3</t>
-  </si>
-  <si>
     <t>E|房间类型-高级|RoomType|High|3</t>
-  </si>
-  <si>
-    <t>E|货币类型-积分|CoinType|Score|3</t>
-  </si>
-  <si>
-    <t>E|游戏类型-德州PLO|GameType|Plo|4</t>
-  </si>
-  <si>
-    <t>E|货币类型-门票|CoinType|Ticket|4</t>
-  </si>
-  <si>
-    <t>E|游戏类型-德州PLO5|GameType|Plo5|5</t>
-  </si>
-  <si>
-    <t>E|游戏类型-德州PLO6|GameType|Plo6|6</t>
-  </si>
-  <si>
-    <t>E|游戏类型-POINTRUMMY|GameType|PR|7</t>
   </si>
   <si>
     <t>@enum:global_enum_cfg|全局枚举表</t>
@@ -1034,13 +1004,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="7" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="3" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="39.75" customWidth="1"/>
     <col min="2" max="2" width="35.375" customWidth="1"/>
@@ -1076,59 +1046,23 @@
       <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2"/>
+      <c r="E2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" t="s">
+    </row>
+    <row r="3" spans="2:5">
+      <c r="B3" t="s">
         <v>9</v>
       </c>
+      <c r="C3"/>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="4" spans="2:2">
+      <c r="B4" t="s">
         <v>11</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1">
-      <c r="A6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1">
-      <c r="A7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1">
-      <c r="A8" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -1154,7 +1088,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>